<commit_message>
small preview of the website + stickers added
</commit_message>
<xml_diff>
--- a/placements (WIP).xlsx
+++ b/placements (WIP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Documents\GitHub\project-newzzztierlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5C94EE-982F-465D-909D-396DD403833B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B36F116-82E7-4BF0-949B-749E2648860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{471EBB6D-7D1B-4A47-A0BC-04B4E692F236}"/>
+    <workbookView xWindow="18855" yWindow="0" windowWidth="10050" windowHeight="15585" xr2:uid="{471EBB6D-7D1B-4A47-A0BC-04B4E692F236}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>STUN</t>
   </si>
   <si>
-    <t>Miyabi(Anomaly, Quickswap); Yixuan(Sheer, Quickswap); Alice(Anomaly, Quickswap);[+1]</t>
-  </si>
-  <si>
     <t>Lighter(Buff);
 Trigger(Aftershock);[+1]</t>
   </si>
@@ -142,9 +139,6 @@
 Yanagi(Anomaly);</t>
   </si>
   <si>
-    <t>Yanagi(Anomaly, Disorder);</t>
-  </si>
-  <si>
     <t>Vivian(Anomaly);
 Orphie(Partner, Aftershock);[+1]</t>
   </si>
@@ -157,6 +151,14 @@
 Ju Fufu(Aftershock, Ult/Chain);
 Lucia(Aftershock, Sheer, HP);
 Yuzuha(Aftershock, Anomaly);</t>
+  </si>
+  <si>
+    <t>Miyabi(Anomaly, Quickswap);
+Yixuan(Sheer, Quickswap);
+Alice(Anomaly, Quickswap);[+1]</t>
+  </si>
+  <si>
+    <t>Yanagi(Anomaly);</t>
   </si>
 </sst>
 </file>
@@ -698,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D142F395-D434-4D84-B664-0BCD4E7D2476}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.28515625" defaultRowHeight="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -730,16 +732,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -747,16 +749,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,16 +766,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -781,11 +783,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -794,12 +796,12 @@
         <v>4</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -807,13 +809,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -822,12 +824,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>